<commit_message>
cleanup, combat updates, more mobs
</commit_message>
<xml_diff>
--- a/combat.xlsx
+++ b/combat.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28780" windowHeight="12390"/>
+    <workbookView xWindow="0" yWindow="920" windowWidth="28780" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>health</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>retaliation</t>
+  </si>
+  <si>
+    <t>armors</t>
+  </si>
+  <si>
+    <t>defense_mob</t>
+  </si>
+  <si>
+    <t>attack_mob</t>
+  </si>
+  <si>
+    <t>levels</t>
+  </si>
+  <si>
+    <t>delay</t>
   </si>
 </sst>
 </file>
@@ -386,15 +401,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:J11"/>
+  <dimension ref="A2:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="12.453125" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D2" t="s">
         <v>9</v>
       </c>
@@ -414,7 +433,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -434,16 +453,16 @@
         <v>13</v>
       </c>
       <c r="J3">
-        <f>(D4 * D7) - (G5 *G6)</f>
-        <v>17.100000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.35">
+        <f>((D4 * D7) * 0.1) - ((G5 * G6) * 0.1)</f>
+        <v>1.3480000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -458,11 +477,11 @@
         <v>14</v>
       </c>
       <c r="J4">
-        <f>((G4*G7) * (D5 * D6) * G11)</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.35">
+        <f>((G4*G7) * 0.8 + (D5 * D6) * G11)</f>
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -479,7 +498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>3</v>
       </c>
@@ -496,7 +515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>4</v>
       </c>
@@ -513,12 +532,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -535,7 +554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>7</v>
       </c>
@@ -552,9 +571,565 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G11">
         <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0.5</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <f>(C16*($D$4* $J$3))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <f>(C17*($D$4* $J$3))</f>
+        <v>10.784000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <f>(C18*($D$4* $J$3))</f>
+        <v>21.568000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <f t="shared" ref="K17:K31" si="0">(C19*($D$4* $J$3))</f>
+        <v>43.136000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>86.272000000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>172.54400000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>215.68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>28</v>
+      </c>
+      <c r="C23">
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>301.952</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>40</v>
+      </c>
+      <c r="C24">
+        <v>40</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>9</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>431.36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>48</v>
+      </c>
+      <c r="C25">
+        <v>48</v>
+      </c>
+      <c r="D25">
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>517.63200000000006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <v>52</v>
+      </c>
+      <c r="C26">
+        <v>52</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>11</v>
+      </c>
+      <c r="F26">
+        <v>11</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>560.76800000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>64</v>
+      </c>
+      <c r="C27">
+        <v>64</v>
+      </c>
+      <c r="D27">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>12</v>
+      </c>
+      <c r="F27">
+        <v>12</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>690.17600000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>78</v>
+      </c>
+      <c r="C28">
+        <v>78</v>
+      </c>
+      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <v>13</v>
+      </c>
+      <c r="F28">
+        <v>13</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>841.15200000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>90</v>
+      </c>
+      <c r="C29">
+        <v>90</v>
+      </c>
+      <c r="D29">
+        <v>13</v>
+      </c>
+      <c r="E29">
+        <v>14</v>
+      </c>
+      <c r="F29">
+        <v>14</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>970.56000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>120</v>
+      </c>
+      <c r="C30">
+        <v>120</v>
+      </c>
+      <c r="D30">
+        <v>14</v>
+      </c>
+      <c r="E30">
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <v>15</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>1294.0800000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>200</v>
+      </c>
+      <c r="C31">
+        <v>200</v>
+      </c>
+      <c r="D31">
+        <v>15</v>
+      </c>
+      <c r="E31">
+        <v>16</v>
+      </c>
+      <c r="F31">
+        <v>16</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>2156.8000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>17</v>
+      </c>
+      <c r="E32">
+        <v>17</v>
+      </c>
+      <c r="F32">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>18</v>
+      </c>
+      <c r="E33">
+        <v>18</v>
+      </c>
+      <c r="F33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>19</v>
+      </c>
+      <c r="E34">
+        <v>19</v>
+      </c>
+      <c r="F34">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>20</v>
+      </c>
+      <c r="E35">
+        <v>20</v>
+      </c>
+      <c r="F35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>21</v>
+      </c>
+      <c r="E36">
+        <v>21</v>
+      </c>
+      <c r="F36">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>22</v>
+      </c>
+      <c r="E37">
+        <v>22</v>
+      </c>
+      <c r="F37">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>23</v>
+      </c>
+      <c r="E38">
+        <v>23</v>
+      </c>
+      <c r="F38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>24</v>
+      </c>
+      <c r="E39">
+        <v>24</v>
+      </c>
+      <c r="F39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>25</v>
+      </c>
+      <c r="E40">
+        <v>25</v>
+      </c>
+      <c r="F40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved combat into its own module. changed combat formulas.
</commit_message>
<xml_diff>
--- a/combat.xlsx
+++ b/combat.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="920" windowWidth="28780" windowHeight="12390"/>
+    <workbookView xWindow="0" yWindow="1380" windowWidth="28780" windowHeight="12390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>health</t>
   </si>
@@ -84,6 +85,33 @@
   </si>
   <si>
     <t>delay</t>
+  </si>
+  <si>
+    <t>[info] combat.round: hit chance calculated 81</t>
+  </si>
+  <si>
+    <t>[info] combat.armor_class: defender armor class is: 2</t>
+  </si>
+  <si>
+    <t>[info] combat.attack: inflicted 10</t>
+  </si>
+  <si>
+    <t>[info] combat.round: hit chance calculated 77</t>
+  </si>
+  <si>
+    <t>[info] combat.armor_class: defender armor class is: 6</t>
+  </si>
+  <si>
+    <t>[info] combat.attack: inflicted 2</t>
+  </si>
+  <si>
+    <t>ac</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>def</t>
   </si>
 </sst>
 </file>
@@ -403,7 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -691,7 +719,7 @@
         <v>4</v>
       </c>
       <c r="K19">
-        <f t="shared" ref="K17:K31" si="0">(C19*($D$4* $J$3))</f>
+        <f t="shared" ref="K19:K31" si="0">(C19*($D$4* $J$3))</f>
         <v>43.136000000000003</v>
       </c>
     </row>
@@ -1130,6 +1158,83 @@
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>